<commit_message>
[week7 day2] math is left
</commit_message>
<xml_diff>
--- a/Personal/xueyu/plan/周计划-2018-03-12.xlsx
+++ b/Personal/xueyu/plan/周计划-2018-03-12.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>今日计划</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -146,6 +146,10 @@
   </si>
   <si>
     <t>高数一节</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yes</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -364,7 +368,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -454,6 +458,93 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -463,12 +554,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="8" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -490,21 +575,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -514,74 +587,8 @@
     <xf numFmtId="9" fontId="4" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="20" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -857,7 +864,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -868,7 +875,7 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -884,23 +891,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="76.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickTop="1">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="69"/>
+      <c r="B2" s="48"/>
       <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
@@ -924,10 +931,10 @@
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="57">
+      <c r="A3" s="45">
         <v>43171</v>
       </c>
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="43" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -939,16 +946,16 @@
         <v>17</v>
       </c>
       <c r="G3" s="20"/>
-      <c r="H3" s="49" t="s">
+      <c r="H3" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="71">
+      <c r="I3" s="50">
         <v>0.8</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="58"/>
-      <c r="B4" s="70"/>
+      <c r="A4" s="46"/>
+      <c r="B4" s="49"/>
       <c r="C4" s="8" t="s">
         <v>11</v>
       </c>
@@ -958,12 +965,12 @@
         <v>17</v>
       </c>
       <c r="G4" s="20"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="72"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="51"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="59"/>
-      <c r="B5" s="67" t="s">
+      <c r="A5" s="44"/>
+      <c r="B5" s="43" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -977,12 +984,12 @@
         <v>17</v>
       </c>
       <c r="G5" s="32"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="72"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="51"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="59"/>
-      <c r="B6" s="59"/>
+      <c r="A6" s="44"/>
+      <c r="B6" s="44"/>
       <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
@@ -992,11 +999,11 @@
         <v>17</v>
       </c>
       <c r="G6" s="33"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="72"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="51"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="59"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="14" t="s">
         <v>15</v>
       </c>
@@ -1011,11 +1018,11 @@
       <c r="G7" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="51"/>
-      <c r="I7" s="73"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="52"/>
     </row>
     <row r="8" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A8" s="77">
+      <c r="A8" s="58">
         <v>43172</v>
       </c>
       <c r="B8" s="60" t="s">
@@ -1025,14 +1032,18 @@
         <v>22</v>
       </c>
       <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="56"/>
+      <c r="E8" s="78">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="57"/>
       <c r="H8" s="13"/>
-      <c r="I8" s="55"/>
+      <c r="I8" s="56"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="56"/>
+      <c r="A9" s="57"/>
       <c r="B9" s="60"/>
       <c r="C9" s="3" t="s">
         <v>23</v>
@@ -1040,13 +1051,13 @@
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
       <c r="F9" s="23"/>
-      <c r="G9" s="56"/>
+      <c r="G9" s="57"/>
       <c r="H9" s="13"/>
-      <c r="I9" s="55"/>
+      <c r="I9" s="56"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="56"/>
-      <c r="B10" s="62" t="s">
+      <c r="A10" s="57"/>
+      <c r="B10" s="61" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1055,26 +1066,28 @@
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
       <c r="F10" s="24"/>
-      <c r="G10" s="56"/>
+      <c r="G10" s="57"/>
       <c r="H10" s="13"/>
-      <c r="I10" s="55"/>
+      <c r="I10" s="56"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="56"/>
-      <c r="B11" s="63"/>
+      <c r="A11" s="57"/>
+      <c r="B11" s="62"/>
       <c r="C11" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D11" s="22"/>
       <c r="E11" s="22"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="56"/>
+      <c r="F11" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="57"/>
       <c r="H11" s="13"/>
-      <c r="I11" s="55"/>
+      <c r="I11" s="56"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="56"/>
-      <c r="B12" s="62" t="s">
+      <c r="A12" s="57"/>
+      <c r="B12" s="61" t="s">
         <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1083,38 +1096,42 @@
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
       <c r="F12" s="24"/>
-      <c r="G12" s="56"/>
+      <c r="G12" s="57"/>
       <c r="H12" s="13"/>
-      <c r="I12" s="55"/>
+      <c r="I12" s="56"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="56"/>
-      <c r="B13" s="64"/>
+      <c r="A13" s="57"/>
+      <c r="B13" s="63"/>
       <c r="C13" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="56"/>
+      <c r="E13" s="78">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="57"/>
       <c r="H13" s="13"/>
-      <c r="I13" s="55"/>
+      <c r="I13" s="56"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="56"/>
-      <c r="B14" s="63"/>
+      <c r="A14" s="57"/>
+      <c r="B14" s="62"/>
       <c r="C14" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
       <c r="F14" s="24"/>
-      <c r="G14" s="56"/>
+      <c r="G14" s="57"/>
       <c r="H14" s="13"/>
-      <c r="I14" s="55"/>
+      <c r="I14" s="56"/>
     </row>
     <row r="15" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A15" s="42"/>
+      <c r="A15" s="69"/>
       <c r="B15" s="10"/>
       <c r="C15" s="1"/>
       <c r="D15" s="25"/>
@@ -1122,43 +1139,43 @@
       <c r="F15" s="26"/>
       <c r="G15" s="26"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="40"/>
+      <c r="I15" s="67"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="43"/>
-      <c r="B16" s="38"/>
+      <c r="A16" s="70"/>
+      <c r="B16" s="59"/>
       <c r="C16" s="5"/>
       <c r="D16" s="26"/>
       <c r="E16" s="26"/>
       <c r="F16" s="26"/>
       <c r="G16" s="26"/>
       <c r="H16" s="5"/>
-      <c r="I16" s="41"/>
+      <c r="I16" s="68"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="43"/>
-      <c r="B17" s="38"/>
+      <c r="A17" s="70"/>
+      <c r="B17" s="59"/>
       <c r="C17" s="1"/>
       <c r="D17" s="26"/>
       <c r="E17" s="18"/>
       <c r="F17" s="26"/>
       <c r="G17" s="26"/>
       <c r="H17" s="5"/>
-      <c r="I17" s="41"/>
+      <c r="I17" s="68"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="43"/>
-      <c r="B18" s="38"/>
+      <c r="A18" s="70"/>
+      <c r="B18" s="59"/>
       <c r="C18" s="1"/>
       <c r="D18" s="26"/>
       <c r="E18" s="26"/>
       <c r="F18" s="26"/>
       <c r="G18" s="26"/>
       <c r="H18" s="5"/>
-      <c r="I18" s="41"/>
+      <c r="I18" s="68"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="43"/>
+      <c r="A19" s="70"/>
       <c r="B19" s="10"/>
       <c r="C19" s="1"/>
       <c r="D19" s="26"/>
@@ -1166,227 +1183,227 @@
       <c r="F19" s="26"/>
       <c r="G19" s="26"/>
       <c r="H19" s="5"/>
-      <c r="I19" s="41"/>
+      <c r="I19" s="68"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="61"/>
-      <c r="B20" s="47"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="36"/>
       <c r="C20" s="9"/>
       <c r="D20" s="27"/>
       <c r="E20" s="27"/>
       <c r="F20" s="27"/>
       <c r="G20" s="27"/>
       <c r="H20" s="6"/>
-      <c r="I20" s="39"/>
+      <c r="I20" s="37"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="61"/>
-      <c r="B21" s="47"/>
+      <c r="A21" s="35"/>
+      <c r="B21" s="36"/>
       <c r="C21" s="9"/>
       <c r="D21" s="27"/>
       <c r="E21" s="27"/>
       <c r="F21" s="27"/>
       <c r="G21" s="27"/>
       <c r="H21" s="6"/>
-      <c r="I21" s="39"/>
+      <c r="I21" s="37"/>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="47"/>
-      <c r="B22" s="47"/>
+      <c r="A22" s="36"/>
+      <c r="B22" s="36"/>
       <c r="C22" s="6"/>
       <c r="D22" s="27"/>
       <c r="E22" s="27"/>
       <c r="F22" s="27"/>
       <c r="G22" s="27"/>
       <c r="H22" s="6"/>
-      <c r="I22" s="39"/>
+      <c r="I22" s="37"/>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="47"/>
-      <c r="B23" s="47"/>
+      <c r="A23" s="36"/>
+      <c r="B23" s="36"/>
       <c r="C23" s="6"/>
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
       <c r="F23" s="27"/>
       <c r="G23" s="27"/>
       <c r="H23" s="6"/>
-      <c r="I23" s="39"/>
+      <c r="I23" s="37"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="47"/>
-      <c r="B24" s="47"/>
+      <c r="A24" s="36"/>
+      <c r="B24" s="36"/>
       <c r="C24" s="6"/>
       <c r="D24" s="27"/>
       <c r="E24" s="27"/>
       <c r="F24" s="27"/>
       <c r="G24" s="27"/>
       <c r="H24" s="6"/>
-      <c r="I24" s="39"/>
+      <c r="I24" s="37"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="47"/>
-      <c r="B25" s="47"/>
+      <c r="A25" s="36"/>
+      <c r="B25" s="36"/>
       <c r="C25" s="6"/>
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
       <c r="F25" s="27"/>
       <c r="G25" s="27"/>
       <c r="H25" s="6"/>
-      <c r="I25" s="39"/>
+      <c r="I25" s="37"/>
     </row>
     <row r="26" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A26" s="44"/>
-      <c r="B26" s="38"/>
+      <c r="A26" s="71"/>
+      <c r="B26" s="59"/>
       <c r="C26" s="7"/>
       <c r="D26" s="28"/>
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="28"/>
-      <c r="H26" s="49"/>
-      <c r="I26" s="52"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="75"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="45"/>
-      <c r="B27" s="38"/>
+      <c r="A27" s="72"/>
+      <c r="B27" s="59"/>
       <c r="C27" s="7"/>
       <c r="D27" s="29"/>
       <c r="E27" s="29"/>
       <c r="F27" s="28"/>
       <c r="G27" s="28"/>
-      <c r="H27" s="50"/>
-      <c r="I27" s="53"/>
+      <c r="H27" s="54"/>
+      <c r="I27" s="76"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="45"/>
-      <c r="B28" s="38"/>
+      <c r="A28" s="72"/>
+      <c r="B28" s="59"/>
       <c r="C28" s="7"/>
       <c r="D28" s="29"/>
       <c r="E28" s="29"/>
       <c r="F28" s="28"/>
       <c r="G28" s="28"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="53"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="76"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="45"/>
-      <c r="B29" s="48"/>
+      <c r="A29" s="72"/>
+      <c r="B29" s="74"/>
       <c r="C29" s="7"/>
       <c r="D29" s="29"/>
       <c r="E29" s="29"/>
       <c r="F29" s="28"/>
       <c r="G29" s="28"/>
-      <c r="H29" s="50"/>
-      <c r="I29" s="53"/>
+      <c r="H29" s="54"/>
+      <c r="I29" s="76"/>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="45"/>
-      <c r="B30" s="48"/>
+      <c r="A30" s="72"/>
+      <c r="B30" s="74"/>
       <c r="C30" s="7"/>
       <c r="D30" s="28"/>
       <c r="E30" s="28"/>
       <c r="F30" s="28"/>
-      <c r="G30" s="35"/>
-      <c r="H30" s="50"/>
-      <c r="I30" s="53"/>
+      <c r="G30" s="64"/>
+      <c r="H30" s="54"/>
+      <c r="I30" s="76"/>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="45"/>
-      <c r="B31" s="48"/>
+      <c r="A31" s="72"/>
+      <c r="B31" s="74"/>
       <c r="C31" s="7"/>
       <c r="D31" s="28"/>
       <c r="E31" s="28"/>
       <c r="F31" s="28"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="50"/>
-      <c r="I31" s="53"/>
+      <c r="G31" s="65"/>
+      <c r="H31" s="54"/>
+      <c r="I31" s="76"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="45"/>
-      <c r="B32" s="48"/>
+      <c r="A32" s="72"/>
+      <c r="B32" s="74"/>
       <c r="C32" s="7"/>
       <c r="D32" s="28"/>
       <c r="E32" s="28"/>
       <c r="F32" s="28"/>
-      <c r="G32" s="37"/>
-      <c r="H32" s="50"/>
-      <c r="I32" s="53"/>
+      <c r="G32" s="66"/>
+      <c r="H32" s="54"/>
+      <c r="I32" s="76"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="46"/>
+      <c r="A33" s="73"/>
       <c r="B33" s="12"/>
       <c r="C33" s="7"/>
       <c r="D33" s="28"/>
       <c r="E33" s="28"/>
       <c r="F33" s="28"/>
       <c r="G33" s="28"/>
-      <c r="H33" s="51"/>
-      <c r="I33" s="54"/>
+      <c r="H33" s="55"/>
+      <c r="I33" s="77"/>
     </row>
     <row r="34" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A34" s="61"/>
-      <c r="B34" s="47"/>
+      <c r="A34" s="35"/>
+      <c r="B34" s="36"/>
       <c r="C34" s="9"/>
       <c r="D34" s="27"/>
       <c r="E34" s="27"/>
       <c r="F34" s="27"/>
       <c r="G34" s="27"/>
-      <c r="H34" s="74"/>
-      <c r="I34" s="39"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="37"/>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="61"/>
-      <c r="B35" s="47"/>
+      <c r="A35" s="35"/>
+      <c r="B35" s="36"/>
       <c r="C35" s="9"/>
       <c r="D35" s="27"/>
       <c r="E35" s="27"/>
       <c r="F35" s="27"/>
       <c r="G35" s="27"/>
-      <c r="H35" s="75"/>
-      <c r="I35" s="39"/>
+      <c r="H35" s="39"/>
+      <c r="I35" s="37"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="47"/>
-      <c r="B36" s="47"/>
+      <c r="A36" s="36"/>
+      <c r="B36" s="36"/>
       <c r="C36" s="6"/>
       <c r="D36" s="27"/>
       <c r="E36" s="27"/>
       <c r="F36" s="27"/>
       <c r="G36" s="27"/>
-      <c r="H36" s="75"/>
-      <c r="I36" s="39"/>
+      <c r="H36" s="39"/>
+      <c r="I36" s="37"/>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="47"/>
-      <c r="B37" s="47"/>
+      <c r="A37" s="36"/>
+      <c r="B37" s="36"/>
       <c r="C37" s="6"/>
       <c r="D37" s="27"/>
       <c r="E37" s="27"/>
       <c r="F37" s="27"/>
       <c r="G37" s="27"/>
-      <c r="H37" s="75"/>
-      <c r="I37" s="39"/>
+      <c r="H37" s="39"/>
+      <c r="I37" s="37"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="47"/>
-      <c r="B38" s="47"/>
+      <c r="A38" s="36"/>
+      <c r="B38" s="36"/>
       <c r="C38" s="6"/>
       <c r="D38" s="27"/>
       <c r="E38" s="27"/>
       <c r="F38" s="27"/>
       <c r="G38" s="27"/>
-      <c r="H38" s="75"/>
-      <c r="I38" s="39"/>
+      <c r="H38" s="39"/>
+      <c r="I38" s="37"/>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="47"/>
-      <c r="B39" s="47"/>
+      <c r="A39" s="36"/>
+      <c r="B39" s="36"/>
       <c r="C39" s="6"/>
       <c r="D39" s="27"/>
       <c r="E39" s="27"/>
       <c r="F39" s="27"/>
       <c r="G39" s="27"/>
-      <c r="H39" s="76"/>
-      <c r="I39" s="39"/>
+      <c r="H39" s="40"/>
+      <c r="I39" s="37"/>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="11"/>
@@ -1544,28 +1561,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A34:A39"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="I34:I39"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="H34:H39"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="I3:I7"/>
-    <mergeCell ref="H3:H7"/>
-    <mergeCell ref="I8:I14"/>
-    <mergeCell ref="G8:G14"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A20:A25"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B14"/>
     <mergeCell ref="G30:G32"/>
     <mergeCell ref="B26:B28"/>
     <mergeCell ref="I20:I25"/>
@@ -1577,6 +1572,28 @@
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="H26:H33"/>
     <mergeCell ref="I26:I33"/>
+    <mergeCell ref="I8:I14"/>
+    <mergeCell ref="G8:G14"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="I3:I7"/>
+    <mergeCell ref="H3:H7"/>
+    <mergeCell ref="A34:A39"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="I34:I39"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="H34:H39"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>